<commit_message>
Actualización imputación de horas
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -361,7 +361,7 @@
       <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.28"/>
@@ -466,11 +466,11 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G7" s="6" t="n">
         <f aca="false">SUM(C7:F7)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>12</v>
@@ -561,11 +561,11 @@
       </c>
       <c r="F13" s="12" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G13" s="12" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Implementación gráficos de horas en excel
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -79,7 +79,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -122,8 +122,18 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,14 +148,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFF3F3F3"/>
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF004586"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF420E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81D41A"/>
+        <bgColor rgb="FF579D1C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF3F3F3"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -225,7 +253,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -250,15 +278,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,7 +314,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -290,7 +330,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFF3F3F3"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -307,11 +347,11 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF3F3F3"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -331,14 +371,14 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FF81D41A"/>
+      <rgbColor rgb="FFFFD320"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF579D1C"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -350,6 +390,1579 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas en el proyecto</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Juan Antonio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Ashley</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Ángela</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Alejandro</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>174600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>27000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>821880</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>3240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8442720" y="5817960"/>
+        <a:ext cx="5762160" cy="3233880"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>105480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>745200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>158760</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8373600" y="2354040"/>
+        <a:ext cx="5754600" cy="3233880"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9360</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>70560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>993600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>50400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2478240" y="5861520"/>
+        <a:ext cx="5760360" cy="3237480"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>429840</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>117000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>970560</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>97200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2455200" y="2469600"/>
+        <a:ext cx="5760360" cy="3237480"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>60480</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>166680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>706320</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="14466600" y="3966840"/>
+        <a:ext cx="5760720" cy="3237480"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -358,10 +1971,10 @@
   <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.28"/>
@@ -436,134 +2049,134 @@
       <c r="H5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6" t="n">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <f aca="false">SUM(C6:F6)</f>
         <v>17</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="n">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="7" t="n">
         <f aca="false">SUM(C7:F7)</f>
         <v>17</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="n">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <f aca="false">SUM(C8:F8)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="n">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="7" t="n">
         <f aca="false">SUM(C9:F9)</f>
         <v>9</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6" t="n">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="n">
         <f aca="false">SUM(C10:F10)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6" t="n">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7" t="n">
         <f aca="false">SUM(C11:F11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="6" t="n">
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="7" t="n">
         <f aca="false">SUM(C12:F12)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="11" t="n">
+      <c r="C13" s="14" t="n">
         <f aca="false">SUM(C6:C12)</f>
         <v>12</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="D13" s="14" t="n">
         <f aca="false">SUM(D6:D12)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="11" t="n">
+      <c r="E13" s="14" t="n">
         <f aca="false">SUM(E6:E9)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="12" t="n">
+      <c r="F13" s="15" t="n">
         <f aca="false">SUM(F6:F12)</f>
         <v>31</v>
       </c>
-      <c r="G13" s="12" t="n">
+      <c r="G13" s="15" t="n">
         <f aca="false">SUM(C13:F13)</f>
         <v>43</v>
       </c>
@@ -8465,5 +10078,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio en las credenciales
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -390,7 +390,1160 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Juan Antonio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$6:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Ashley</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$6:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Ángela</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas Alejandro</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="none"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -508,6 +1661,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -528,6 +1682,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -548,6 +1703,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -568,6 +1724,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -586,6 +1743,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="bestFit"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -621,10 +1779,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -667,1135 +1825,7 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas Juan Antonio</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$6:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas Ashley</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$6:$F$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas Ángela</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$6:$D$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas Alejandro</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="none"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$E$6:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1819,9 +1849,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>821880</xdr:colOff>
+      <xdr:colOff>821160</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1829,8 +1859,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8442720" y="5817960"/>
-        <a:ext cx="5762160" cy="3233880"/>
+        <a:off x="8450280" y="5817960"/>
+        <a:ext cx="5774400" cy="3233160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1849,9 +1879,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>745200</xdr:colOff>
+      <xdr:colOff>744480</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>158760</xdr:rowOff>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1859,8 +1889,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8373600" y="2354040"/>
-        <a:ext cx="5754600" cy="3233880"/>
+        <a:off x="8381160" y="2354040"/>
+        <a:ext cx="5766840" cy="3233160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1879,9 +1909,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>993600</xdr:colOff>
+      <xdr:colOff>992880</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>49680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1890,7 +1920,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2478240" y="5861520"/>
-        <a:ext cx="5760360" cy="3237480"/>
+        <a:ext cx="5765040" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1909,9 +1939,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>970560</xdr:colOff>
+      <xdr:colOff>969840</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1920,7 +1950,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2455200" y="2469600"/>
-        <a:ext cx="5760360" cy="3237480"/>
+        <a:ext cx="5765040" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1939,9 +1969,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>706320</xdr:colOff>
+      <xdr:colOff>705600</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1949,8 +1979,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14466600" y="3966840"/>
-        <a:ext cx="5760720" cy="3237480"/>
+        <a:off x="14489280" y="3966840"/>
+        <a:ext cx="5772960" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1971,10 +2001,10 @@
   <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.28"/>
@@ -2059,11 +2089,11 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G6" s="7" t="n">
         <f aca="false">SUM(C6:F6)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>10</v>
@@ -2079,11 +2109,11 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G7" s="7" t="n">
         <f aca="false">SUM(C7:F7)</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>12</v>
@@ -2174,11 +2204,11 @@
       </c>
       <c r="F13" s="15" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G13" s="15" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Cambio estructura avatar y solución compra en API
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -425,408 +425,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas en el proyecto</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web Base de datos Despliegue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Base de datos</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Despliegue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$6:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1215,7 +814,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1548,10 +1147,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1610,7 +1209,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1999,7 +1598,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2391,6 +1990,407 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas en el proyecto</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web Base de datos Despliegue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Base de datos</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Despliegue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2402,9 +2402,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>819720</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>819360</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>176040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2412,8 +2412,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8461800" y="5635080"/>
-        <a:ext cx="5798160" cy="3128760"/>
+        <a:off x="8465760" y="5635080"/>
+        <a:ext cx="5803920" cy="3128400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2432,9 +2432,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>743040</xdr:colOff>
+      <xdr:colOff>742680</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2442,8 +2442,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8392680" y="2279520"/>
-        <a:ext cx="5790600" cy="3134880"/>
+        <a:off x="8396640" y="2279520"/>
+        <a:ext cx="5796360" cy="3134520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2462,9 +2462,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>991440</xdr:colOff>
+      <xdr:colOff>991080</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2473,7 +2473,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2468520" y="5678640"/>
-        <a:ext cx="5779440" cy="3132360"/>
+        <a:ext cx="5781600" cy="3132000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2492,9 +2492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>968400</xdr:colOff>
+      <xdr:colOff>968040</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>95040</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2503,7 +2503,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2450160" y="2395080"/>
-        <a:ext cx="5774760" cy="3132720"/>
+        <a:ext cx="5776920" cy="3132360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2522,9 +2522,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>704160</xdr:colOff>
+      <xdr:colOff>703800</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2532,8 +2532,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14531400" y="3846960"/>
-        <a:ext cx="5796720" cy="3132360"/>
+        <a:off x="14542920" y="3846960"/>
+        <a:ext cx="5802480" cy="3132000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2553,11 +2553,11 @@
   </sheetPr>
   <dimension ref="A1:I999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.22"/>
@@ -2646,11 +2646,11 @@
         <v>3</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G6" s="7" t="n">
         <f aca="false">SUM(C6:F6)</f>
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>10</v>
@@ -2666,11 +2666,11 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G7" s="7" t="n">
         <f aca="false">SUM(C7:F7)</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>12</v>
@@ -2771,11 +2771,11 @@
       </c>
       <c r="F13" s="17" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G13" s="17" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Solución web función comprar
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -85,7 +85,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -118,6 +118,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -280,7 +288,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -325,11 +333,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1152,11 +1164,8 @@
                 <c:pt idx="1">
                   <c:v>22</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,7 +2341,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2402,9 +2411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>819360</xdr:colOff>
+      <xdr:colOff>818280</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>176040</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2412,8 +2421,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8465760" y="5635080"/>
-        <a:ext cx="5803920" cy="3128400"/>
+        <a:off x="8476920" y="5635080"/>
+        <a:ext cx="5822280" cy="3127320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2432,9 +2441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>742680</xdr:colOff>
+      <xdr:colOff>741600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2442,8 +2451,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8396640" y="2279520"/>
-        <a:ext cx="5796360" cy="3134520"/>
+        <a:off x="8407800" y="2279520"/>
+        <a:ext cx="5814720" cy="3133440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2462,9 +2471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>991080</xdr:colOff>
+      <xdr:colOff>990000</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>46800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2473,7 +2482,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2468520" y="5678640"/>
-        <a:ext cx="5781600" cy="3132000"/>
+        <a:ext cx="5788080" cy="3130920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2492,9 +2501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>968040</xdr:colOff>
+      <xdr:colOff>966960</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>93600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2503,7 +2512,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2450160" y="2395080"/>
-        <a:ext cx="5776920" cy="3132360"/>
+        <a:ext cx="5783400" cy="3131280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2522,9 +2531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>703800</xdr:colOff>
+      <xdr:colOff>702720</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2532,8 +2541,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14542920" y="3846960"/>
-        <a:ext cx="5802480" cy="3132000"/>
+        <a:off x="14577120" y="3846960"/>
+        <a:ext cx="5820480" cy="3130920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2551,13 +2560,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I999"/>
+  <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.22"/>
@@ -2683,17 +2692,16 @@
       <c r="C8" s="4"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
-      <c r="F8" s="7" t="n">
-        <v>0</v>
-      </c>
+      <c r="F8" s="7"/>
       <c r="G8" s="7" t="n">
         <f aca="false">SUM(C8:F8)</f>
         <v>0</v>
       </c>
       <c r="H8" s="7"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="4" t="n">
@@ -2706,16 +2714,16 @@
         <v>7</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G9" s="7" t="n">
         <f aca="false">SUM(C9:F9)</f>
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="4"/>
@@ -2729,7 +2737,7 @@
       <c r="H10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="4"/>
@@ -2743,39 +2751,39 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="7" t="n">
         <f aca="false">SUM(C12:F12)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="15"/>
+      <c r="H12" s="16"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="16" t="n">
+      <c r="C13" s="17" t="n">
         <f aca="false">SUM(C6:C12)</f>
         <v>37</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="17" t="n">
         <f aca="false">SUM(D6:D12)</f>
         <v>29</v>
       </c>
-      <c r="E13" s="16" t="n">
+      <c r="E13" s="17" t="n">
         <f aca="false">SUM(E6:E9)</f>
         <v>28</v>
       </c>
-      <c r="F13" s="17" t="n">
+      <c r="F13" s="18" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>47</v>
+        <v>52</v>
       </c>
-      <c r="G13" s="17" t="n">
+      <c r="G13" s="18" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Tienda web automatizada y compra implemetnada
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -437,7 +437,408 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas en el proyecto</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web Base de datos Despliegue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Base de datos</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Despliegue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -826,7 +1227,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1162,10 +1563,10 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1218,7 +1619,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1607,7 +2008,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1999,407 +2400,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas en el proyecto</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web Base de datos Despliegue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Base de datos</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Despliegue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$6:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2411,9 +2411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>818280</xdr:colOff>
+      <xdr:colOff>817560</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2421,8 +2421,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8476920" y="5635080"/>
-        <a:ext cx="5822280" cy="3127320"/>
+        <a:off x="8484840" y="5635080"/>
+        <a:ext cx="5833800" cy="3126600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2441,9 +2441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>741600</xdr:colOff>
+      <xdr:colOff>740880</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2451,8 +2451,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8407800" y="2279520"/>
-        <a:ext cx="5814720" cy="3133440"/>
+        <a:off x="8415720" y="2279520"/>
+        <a:ext cx="5826240" cy="3132720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2471,9 +2471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>990000</xdr:colOff>
+      <xdr:colOff>989280</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>46800</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2482,7 +2482,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2468520" y="5678640"/>
-        <a:ext cx="5788080" cy="3130920"/>
+        <a:ext cx="5792760" cy="3130200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2501,9 +2501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>966960</xdr:colOff>
+      <xdr:colOff>966240</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:rowOff>92880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2512,7 +2512,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2450160" y="2395080"/>
-        <a:ext cx="5783400" cy="3131280"/>
+        <a:ext cx="5788080" cy="3130560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2525,15 +2525,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>60480</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:colOff>60840</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>702720</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>142920</xdr:rowOff>
+      <xdr:colOff>702360</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2541,8 +2541,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14577120" y="3846960"/>
-        <a:ext cx="5820480" cy="3130920"/>
+        <a:off x="14600160" y="3933720"/>
+        <a:ext cx="5832720" cy="3130200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2562,11 +2562,11 @@
   </sheetPr>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.6953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.73046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.22"/>
@@ -2675,11 +2675,11 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G7" s="7" t="n">
         <f aca="false">SUM(C7:F7)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>12</v>
@@ -2714,11 +2714,11 @@
         <v>7</v>
       </c>
       <c r="F9" s="7" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G9" s="7" t="n">
         <f aca="false">SUM(C9:F9)</f>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H9" s="7"/>
     </row>
@@ -2779,11 +2779,11 @@
       </c>
       <c r="F13" s="18" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G13" s="18" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Implementación servicio partida y servicio avatar para ajustes de usuario
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -437,408 +437,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Imputación de horas en el proyecto</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>API REST Android Unity Web Base de datos Despliegue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:explosion val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="3"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="579d1c"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="7e0021"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="83caff"/>
-              </a:solidFill>
-              <a:ln w="0">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-          </c:dPt>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="5"/>
-              <c:txPr>
-                <a:bodyPr wrap="square"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:latin typeface="Arial"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:separator> </c:separator>
-            </c:dLbl>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="bestFit"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$6:$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>API REST</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Android</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Unity</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Web</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Base de datos</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Despliegue</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$G$6:$G$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1227,7 +826,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1560,10 +1159,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -1619,7 +1218,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2008,7 +1607,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2400,6 +1999,407 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" lang="ca-ES" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Imputación de horas en el proyecto</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>API REST Android Unity Web Base de datos Despliegue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:explosion val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="579d1c"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln w="0">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:txPr>
+                <a:bodyPr wrap="square"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Arial"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:separator> </c:separator>
+            </c:dLbl>
+            <c:txPr>
+              <a:bodyPr wrap="square"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="bestFit"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$6:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>API REST</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Android</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unity</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Base de datos</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Despliegue</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$6:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="ca-ES" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -2411,9 +2411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>816840</xdr:colOff>
+      <xdr:colOff>816480</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>173520</xdr:rowOff>
+      <xdr:rowOff>173160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2421,8 +2421,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8492400" y="5635080"/>
-        <a:ext cx="5846040" cy="3125880"/>
+        <a:off x="8496000" y="5635080"/>
+        <a:ext cx="5852160" cy="3125520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2441,9 +2441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>740160</xdr:colOff>
+      <xdr:colOff>739800</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2451,8 +2451,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8423280" y="2279520"/>
-        <a:ext cx="5838480" cy="3132000"/>
+        <a:off x="8426880" y="2279520"/>
+        <a:ext cx="5844600" cy="3131640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2471,9 +2471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>988560</xdr:colOff>
+      <xdr:colOff>988200</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2482,7 +2482,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2468520" y="5678640"/>
-        <a:ext cx="5797080" cy="3129480"/>
+        <a:ext cx="5799240" cy="3129120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2501,9 +2501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>965520</xdr:colOff>
+      <xdr:colOff>965160</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>92160</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2512,7 +2512,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2450160" y="2395080"/>
-        <a:ext cx="5792400" cy="3129840"/>
+        <a:ext cx="5794560" cy="3129480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2531,9 +2531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>701640</xdr:colOff>
+      <xdr:colOff>701280</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2541,8 +2541,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14623200" y="3933720"/>
-        <a:ext cx="5844600" cy="3129480"/>
+        <a:off x="14634720" y="3933720"/>
+        <a:ext cx="5850360" cy="3129120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2563,10 +2563,10 @@
   <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.76953125" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.22"/>
@@ -2655,11 +2655,11 @@
         <v>3</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G6" s="7" t="n">
         <f aca="false">SUM(C6:F6)</f>
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>10</v>
@@ -2675,11 +2675,11 @@
         <v>18</v>
       </c>
       <c r="F7" s="7" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" s="7" t="n">
         <f aca="false">SUM(C7:F7)</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>12</v>
@@ -2779,11 +2779,11 @@
       </c>
       <c r="F13" s="18" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G13" s="18" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Solución error Partida Service
</commit_message>
<xml_diff>
--- a/imputacioHoresDSA.xlsx
+++ b/imputacioHoresDSA.xlsx
@@ -437,7 +437,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -826,7 +826,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1159,7 +1159,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
@@ -1218,7 +1218,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1607,7 +1607,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1999,7 +1999,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2332,7 +2332,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>48</c:v>
@@ -2411,9 +2411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>816480</xdr:colOff>
+      <xdr:colOff>816120</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2421,8 +2421,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8496000" y="5635080"/>
-        <a:ext cx="5852160" cy="3125520"/>
+        <a:off x="8499960" y="5635080"/>
+        <a:ext cx="5857920" cy="3125160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2441,9 +2441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>739800</xdr:colOff>
+      <xdr:colOff>739440</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2451,8 +2451,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8426880" y="2279520"/>
-        <a:ext cx="5844600" cy="3131640"/>
+        <a:off x="8430840" y="2279520"/>
+        <a:ext cx="5850360" cy="3131280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2471,9 +2471,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>988200</xdr:colOff>
+      <xdr:colOff>987840</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>45000</xdr:rowOff>
+      <xdr:rowOff>44640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2482,7 +2482,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2468520" y="5678640"/>
-        <a:ext cx="5799240" cy="3129120"/>
+        <a:ext cx="5801400" cy="3128760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2501,9 +2501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>965160</xdr:colOff>
+      <xdr:colOff>964800</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2512,7 +2512,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2450160" y="2395080"/>
-        <a:ext cx="5794560" cy="3129480"/>
+        <a:ext cx="5796720" cy="3129120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2531,9 +2531,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>701280</xdr:colOff>
+      <xdr:colOff>700920</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>52560</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2541,8 +2541,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14634720" y="3933720"/>
-        <a:ext cx="5850360" cy="3129120"/>
+        <a:off x="14645880" y="3933720"/>
+        <a:ext cx="5856840" cy="3128760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2562,11 +2562,11 @@
   </sheetPr>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.22"/>
@@ -2655,11 +2655,11 @@
         <v>3</v>
       </c>
       <c r="F6" s="7" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="7" t="n">
         <f aca="false">SUM(C6:F6)</f>
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>10</v>
@@ -2779,11 +2779,11 @@
       </c>
       <c r="F13" s="18" t="n">
         <f aca="false">SUM(F6:F12)</f>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G13" s="18" t="n">
         <f aca="false">SUM(C13:F13)</f>
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H13" s="1"/>
     </row>

</xml_diff>